<commit_message>
Hell yeah! Recuperação de erro com heurística.
</commit_message>
<xml_diff>
--- a/first_follow.xlsx
+++ b/first_follow.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>Símbolo</t>
   </si>
@@ -29,15 +29,6 @@
     <t>program</t>
   </si>
   <si>
-    <t>decl-list-tail</t>
-  </si>
-  <si>
-    <t>decl</t>
-  </si>
-  <si>
-    <t>ident-list</t>
-  </si>
-  <si>
     <t>ident-list-tail</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>or, +, -</t>
   </si>
   <si>
-    <t>&gt;, =, &gt;=, &lt;. &lt;=, &lt;&gt;</t>
-  </si>
-  <si>
     <t>id, num, (, not, -</t>
   </si>
   <si>
@@ -143,9 +131,6 @@
     <t>or, +, -, λ</t>
   </si>
   <si>
-    <t>&gt;, =, &gt;=, &lt;. &lt;=, &lt;&gt;, λ</t>
-  </si>
-  <si>
     <t>write</t>
   </si>
   <si>
@@ -179,9 +164,6 @@
     <t>",", λ</t>
   </si>
   <si>
-    <t>id, λ</t>
-  </si>
-  <si>
     <t>$</t>
   </si>
   <si>
@@ -218,15 +200,6 @@
     <t>)</t>
   </si>
   <si>
-    <t>;, ), &gt;, =, &gt;=, &lt;. &lt;=, &lt;&gt;</t>
-  </si>
-  <si>
-    <t>or, +, -, ;, ), &gt;, =, &gt;=, &lt;. &lt;=, &lt;&gt;</t>
-  </si>
-  <si>
-    <t>*, /, and, or, +, -, ;, ), &gt;, =, &gt;=, &lt;. &lt;=, &lt;&gt;</t>
-  </si>
-  <si>
     <t>num, string</t>
   </si>
   <si>
@@ -237,6 +210,21 @@
   </si>
   <si>
     <t>decl-stmt-list-tail</t>
+  </si>
+  <si>
+    <t>&gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;, λ</t>
+  </si>
+  <si>
+    <t>;, ), &gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;</t>
+  </si>
+  <si>
+    <t>or, +, -, ;, ), &gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;</t>
+  </si>
+  <si>
+    <t>*, /, and, or, +, -, ;, ), &gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;</t>
+  </si>
+  <si>
+    <t>&gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -578,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,10 +584,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,54 +595,54 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,10 +650,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,10 +661,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,10 +672,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,10 +683,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,10 +694,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,10 +705,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,10 +716,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,10 +727,10 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -750,10 +738,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,10 +749,10 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,10 +760,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,10 +771,10 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,10 +782,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -805,10 +793,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,10 +804,10 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -827,10 +815,10 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -838,7 +826,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
         <v>64</v>
@@ -849,7 +837,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>64</v>
@@ -860,10 +848,10 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,7 +859,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
         <v>65</v>
@@ -882,10 +870,10 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,7 +881,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
         <v>66</v>
@@ -904,10 +892,10 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -915,10 +903,10 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,10 +914,10 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -937,43 +925,10 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>